<commit_message>
add domain model diagram generator
</commit_message>
<xml_diff>
--- a/business-events_object-model-changes.xlsx
+++ b/business-events_object-model-changes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martin/stuff/objectmodeldiagramgenerator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C0D03C9-03AD-E045-AEE7-35B8B79E5FD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9197D26-FBA3-ED49-AB62-A02B31023996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="11740" activeTab="1" xr2:uid="{EA4244F2-FE33-7643-A566-43DD5B4E5092}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="60">
   <si>
     <t>ID</t>
   </si>
@@ -93,9 +93,6 @@
     <t>DE_IBPIN</t>
   </si>
   <si>
-    <t>zuda0001_ib</t>
-  </si>
-  <si>
     <t>Anton Anfang enrolls B2G for his Zugang</t>
   </si>
   <si>
@@ -204,9 +201,6 @@
     <t>CTR_P</t>
   </si>
   <si>
-    <t>ING</t>
-  </si>
-  <si>
     <t>apro0001</t>
   </si>
   <si>
@@ -217,6 +211,9 @@
   </si>
   <si>
     <t>uuid_pk</t>
+  </si>
+  <si>
+    <t>ING0001</t>
   </si>
 </sst>
 </file>
@@ -446,33 +443,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -481,6 +451,33 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -851,7 +848,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -859,7 +856,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -867,7 +864,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
         <v>14</v>
@@ -875,10 +872,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -892,10 +889,10 @@
   <dimension ref="A1:AD8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="O4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="Z4" sqref="Z4"/>
+      <selection pane="bottomRight" activeCell="AA7" sqref="AA7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -907,456 +904,456 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" s="9" customFormat="1" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="12" t="s">
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
-      <c r="T1" s="13"/>
-      <c r="U1" s="13"/>
-      <c r="V1" s="13"/>
-      <c r="W1" s="13"/>
-      <c r="X1" s="13"/>
-      <c r="Y1" s="13"/>
-      <c r="Z1" s="13"/>
-      <c r="AA1" s="13"/>
-      <c r="AB1" s="13"/>
-      <c r="AC1" s="13"/>
-      <c r="AD1" s="13"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+      <c r="W1" s="22"/>
+      <c r="X1" s="22"/>
+      <c r="Y1" s="22"/>
+      <c r="Z1" s="22"/>
+      <c r="AA1" s="22"/>
+      <c r="AB1" s="22"/>
+      <c r="AC1" s="22"/>
+      <c r="AD1" s="22"/>
     </row>
     <row r="2" spans="1:30" s="9" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="22"/>
-      <c r="B2" s="19" t="s">
+      <c r="A2" s="13"/>
+      <c r="B2" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="16"/>
+      <c r="D2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" s="15"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="L2" s="16"/>
+      <c r="M2" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="N2" s="18"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q2" s="18"/>
+      <c r="R2" s="18"/>
+      <c r="S2" s="19"/>
+      <c r="T2" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="I2" s="19"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="L2" s="18"/>
-      <c r="M2" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="N2" s="15"/>
-      <c r="O2" s="16"/>
-      <c r="P2" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="15"/>
-      <c r="S2" s="16"/>
-      <c r="T2" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="U2" s="15"/>
-      <c r="V2" s="15"/>
-      <c r="W2" s="16"/>
-      <c r="X2" s="14" t="s">
+      <c r="U2" s="18"/>
+      <c r="V2" s="18"/>
+      <c r="W2" s="19"/>
+      <c r="X2" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y2" s="19"/>
+      <c r="Z2" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="Y2" s="16"/>
-      <c r="Z2" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="AA2" s="15"/>
-      <c r="AB2" s="15"/>
-      <c r="AC2" s="15"/>
-      <c r="AD2" s="15"/>
+      <c r="AA2" s="18"/>
+      <c r="AB2" s="18"/>
+      <c r="AC2" s="18"/>
+      <c r="AD2" s="18"/>
     </row>
     <row r="3" spans="1:30" s="9" customFormat="1" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="23"/>
+      <c r="A3" s="14"/>
       <c r="B3" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="K3" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="N3" s="7" t="s">
         <v>9</v>
       </c>
       <c r="O3" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Q3" s="7" t="s">
         <v>11</v>
       </c>
       <c r="R3" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="S3" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="S3" s="7" t="s">
-        <v>50</v>
-      </c>
       <c r="T3" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="U3" s="7" t="s">
         <v>11</v>
       </c>
       <c r="V3" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="W3" s="8" t="s">
         <v>15</v>
       </c>
       <c r="X3" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Y3" s="8" t="s">
         <v>11</v>
       </c>
       <c r="Z3" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AA3" s="7" t="s">
         <v>11</v>
       </c>
       <c r="AB3" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AC3" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AD3" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K4" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L4" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M4" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N4" s="10" t="s">
         <v>5</v>
       </c>
       <c r="O4" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="P4" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q4" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="R4" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="P4" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q4" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="R4" s="10" t="s">
-        <v>25</v>
-      </c>
       <c r="S4" s="10" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="T4" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="U4" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="V4" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="W4" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="X4" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Y4" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Z4" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AA4" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AB4" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AC4" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AD4" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D5" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="10" t="s">
         <v>32</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>33</v>
       </c>
       <c r="F5" s="10" t="s">
         <v>12</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L5" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M5" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N5" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O5" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="P5" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Q5" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="R5" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="S5" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="T5" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="U5" s="10" t="s">
         <v>13</v>
       </c>
       <c r="V5" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="W5" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="X5" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Y5" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Z5" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AA5" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AB5" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AC5" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AD5" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H6" s="10" t="s">
         <v>16</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K6" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L6" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M6" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N6" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O6" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="P6" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Q6" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="R6" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="S6" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="T6" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="U6" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="V6" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="W6" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="X6" s="10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="Y6" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="Z6" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AA6" s="10" t="s">
         <v>17</v>
       </c>
       <c r="AB6" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AC6" s="10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="AD6" s="10" t="s">
         <v>16</v>
@@ -1364,186 +1361,186 @@
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I7" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L7" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M7" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N7" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O7" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="P7" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Q7" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="R7" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="S7" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="T7" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="U7" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="V7" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="W7" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="X7" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Y7" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Z7" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AA7" s="10" t="s">
         <v>18</v>
       </c>
       <c r="AB7" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AC7" s="10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="AD7" s="10" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I8" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K8" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L8" s="10" t="s">
         <v>16</v>
       </c>
       <c r="M8" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N8" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O8" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="P8" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Q8" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="R8" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="S8" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="T8" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="U8" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="V8" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="W8" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="X8" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Y8" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Z8" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AA8" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB8" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="AC8" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD8" s="10" t="s">
         <v>22</v>
-      </c>
-      <c r="AB8" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="AC8" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD8" s="10" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>